<commit_message>
Updated SUPPLY - minor changes to HVAC
Changed some values, added a reference for "Germany" in EUR 2015 (danish energy agency technology database)
</commit_message>
<xml_diff>
--- a/cea/databases/DE/assemblies/HVAC.xlsx
+++ b/cea/databases/DE/assemblies/HVAC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge38yoz\cea-tests\databases\2024-02-08_DE\assemblies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge38yoz\CityEnergyAnalyst\cea\databases\DE\assemblies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601CAAE6-EDE3-412C-B259-5AD5E90F0BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E649D94-670D-43B4-8CC2-81815F3428BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16410" yWindow="7335" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HOT_WATER" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,20 @@
     <sheet name="VENTILATION" sheetId="4" r:id="rId4"/>
     <sheet name="CONTROLLER" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -486,16 +499,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -510,16 +520,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -799,16 +803,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -819,7 +823,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -833,13 +837,13 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>0</v>
       </c>
       <c r="E2" s="3">
@@ -850,13 +854,13 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>60</v>
       </c>
       <c r="E3" s="3">
@@ -867,13 +871,13 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>45</v>
       </c>
       <c r="E4" s="3">
@@ -884,13 +888,13 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>35</v>
       </c>
       <c r="E5" s="3">
@@ -901,13 +905,13 @@
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>60</v>
       </c>
       <c r="E6" s="3">
@@ -924,18 +928,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -990,43 +994,43 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="8">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1034,43 +1038,43 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
         <v>500</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.15</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="3">
         <v>90</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>20</v>
       </c>
     </row>
@@ -1078,43 +1082,43 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>500</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>-0.1</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="4">
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="3">
         <v>70</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>15</v>
       </c>
     </row>
@@ -1122,43 +1126,43 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>500</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>40</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>20</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>36</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>40</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>20</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>36</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="M5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1166,43 +1170,43 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>0.5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>150</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>-0.9</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="4">
+      <c r="G6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="3">
         <v>40</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1221,7 +1225,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -1290,43 +1294,43 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="8">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1334,43 +1338,43 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>500</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>0.5</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="3">
         <v>18</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1378,43 +1382,43 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>150</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>0.7</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3">
         <v>7.5</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>7</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>16</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="M4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1422,57 +1426,57 @@
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>500</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0.5</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>7.5</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>7</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>16</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>7.5</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>7</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>16</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="M5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="E6" s="3">
@@ -1510,43 +1514,43 @@
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>0.1</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>100</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>0.5</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="4">
+      <c r="G7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="3">
         <v>18</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1564,9 +1568,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1602,7 +1606,7 @@
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="2" t="b">
@@ -1625,7 +1629,7 @@
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C3" s="2" t="b">
@@ -1648,7 +1652,7 @@
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="2" t="b">
@@ -1668,10 +1672,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>73</v>
       </c>
       <c r="C5" s="2" t="b">
@@ -1703,7 +1707,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
@@ -1727,7 +1731,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C2" s="3">
@@ -1741,7 +1745,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="3">
@@ -1755,7 +1759,7 @@
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C4" s="3">
@@ -1769,7 +1773,7 @@
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C5" s="3">
@@ -1783,7 +1787,7 @@
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="3">

</xml_diff>